<commit_message>
memperbaiki logika untuk menyimpan multiple data dan memperbaiki tabel angsuran
</commit_message>
<xml_diff>
--- a/database/data/demoLoan.xlsx
+++ b/database/data/demoLoan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20406"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projek Sekolah\koperasi-api\database\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIN WEB\GIN WEB\project\Koperasi App\koperasi-api\database\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E350B4-7CCE-49C1-9F78-13037A98F2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7499F7D2-7ABA-4F80-80E8-04897941130F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{49AD8E68-4375-4243-8469-847B5B5DBAF5}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" xr2:uid="{49AD8E68-4375-4243-8469-847B5B5DBAF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,21 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>member</t>
   </si>
@@ -72,28 +63,34 @@
     <t>Tini</t>
   </si>
   <si>
-    <t>pinjaman mandiri</t>
-  </si>
-  <si>
-    <t>berjalan</t>
-  </si>
-  <si>
-    <t>lunas</t>
-  </si>
-  <si>
     <t>belum bayar</t>
   </si>
   <si>
     <t>deadline</t>
   </si>
   <si>
-    <t>30-05-2023</t>
-  </si>
-  <si>
-    <t>30-10-2023</t>
-  </si>
-  <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>piutang s/p</t>
+  </si>
+  <si>
+    <t>MARIAM HIDAYAT, S.Pd</t>
+  </si>
+  <si>
+    <t>piutang dagang</t>
+  </si>
+  <si>
+    <t>30-10-2024</t>
+  </si>
+  <si>
+    <t>30-12-2024</t>
+  </si>
+  <si>
+    <t>08-09-2024</t>
+  </si>
+  <si>
+    <t>08-12-2024</t>
   </si>
 </sst>
 </file>
@@ -129,9 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -446,27 +445,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D572EF84-00F9-41FD-8FAF-04CB0554CFE5}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" customWidth="1"/>
-    <col min="4" max="4" width="17.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" customWidth="1"/>
     <col min="8" max="8" width="21" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.77734375" customWidth="1"/>
+    <col min="9" max="10" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -486,7 +484,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -498,36 +496,36 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
-        <v>1000000</v>
+        <v>10000000</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E2">
         <v>1.5</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H2">
-        <v>1015000</v>
+        <v>11500000</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -535,7 +533,7 @@
         <v>50000000</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -544,48 +542,74 @@
         <v>1.5</v>
       </c>
       <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3">
+        <v>57500000</v>
+      </c>
+      <c r="I3" t="s">
         <v>14</v>
       </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3">
-        <v>50750000</v>
-      </c>
-      <c r="I3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" t="s">
-        <v>18</v>
-      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
-        <v>500000</v>
+        <v>20000000</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E4">
         <v>1.5</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
       </c>
       <c r="H4">
-        <v>507500</v>
+        <v>21500000</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>5000000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>1.5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>7250000</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>